<commit_message>
includes changes to Loopback  docs page
</commit_message>
<xml_diff>
--- a/docs/source/hardware/loopback_PCB/connectors.xlsx
+++ b/docs/source/hardware/loopback_PCB/connectors.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ultrazohm_sw\docs\source\hardware\loopback_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D6790AE-8ED0-40CE-81FB-492EB52F2C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0FF1151-E54F-440D-9B1D-8D8A1794D9F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="108">
   <si>
     <t>Pin</t>
   </si>
@@ -135,9 +146,6 @@
     <t>IO_P7</t>
   </si>
   <si>
-    <t>/</t>
-  </si>
-  <si>
     <t>DIG_IO_P14</t>
   </si>
   <si>
@@ -259,13 +267,106 @@
   </si>
   <si>
     <t>DIG_IO_P1</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>LED_G1_D6</t>
+  </si>
+  <si>
+    <t>LED_G7_D6</t>
+  </si>
+  <si>
+    <t>LED_G2_D6</t>
+  </si>
+  <si>
+    <t>LED_G9_D6</t>
+  </si>
+  <si>
+    <t>LED_G3_D6</t>
+  </si>
+  <si>
+    <t>LED_G10_D6</t>
+  </si>
+  <si>
+    <t>LED1_D5</t>
+  </si>
+  <si>
+    <t>LED2_D5</t>
+  </si>
+  <si>
+    <t>LED3_D5</t>
+  </si>
+  <si>
+    <t>LED4_D5</t>
+  </si>
+  <si>
+    <t>LED5_D5</t>
+  </si>
+  <si>
+    <t>LED6_D5</t>
+  </si>
+  <si>
+    <t>LED7_D5</t>
+  </si>
+  <si>
+    <t>LED_G4_D6</t>
+  </si>
+  <si>
+    <t>LED_G8_D6</t>
+  </si>
+  <si>
+    <t>LED_G5_D6</t>
+  </si>
+  <si>
+    <t>LED_G11_D6</t>
+  </si>
+  <si>
+    <t>LED_G6_D6</t>
+  </si>
+  <si>
+    <t>LED_G12_D6</t>
+  </si>
+  <si>
+    <t>LED8_D5</t>
+  </si>
+  <si>
+    <t>LED9_D5</t>
+  </si>
+  <si>
+    <t>LED10_D5</t>
+  </si>
+  <si>
+    <t>LED11_D5</t>
+  </si>
+  <si>
+    <t>LED12_D5</t>
+  </si>
+  <si>
+    <t>LED13_D5</t>
+  </si>
+  <si>
+    <t>LED14_D5</t>
+  </si>
+  <si>
+    <t>LED15_D5</t>
+  </si>
+  <si>
+    <t>LED16_D5</t>
+  </si>
+  <si>
+    <t>LED17_D5</t>
+  </si>
+  <si>
+    <t>LED18_D5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -285,6 +386,12 @@
       <color rgb="FF404040"/>
       <name val="Lato"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -307,7 +414,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -367,11 +474,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFE1E4E5"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -389,6 +505,12 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -671,18 +793,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G1" sqref="G1:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="15.7109375" customWidth="1"/>
+    <col min="1" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="81" customWidth="1"/>
+    <col min="8" max="12" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="102.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -692,8 +817,15 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
+      </c>
+      <c r="G1" t="str">
+        <f>_xlfn.CONCAT(A1,",",B1,",",C1,",",D1,",",E1)</f>
+        <v>Pin,Digital voltage card,Loopback PCB,LED,ADC card</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>0</v>
@@ -704,11 +836,18 @@
       <c r="K1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P1" s="8" t="str">
+        <f>_xlfn.CONCAT(I1,",",J1,",",K1,",",L1,",",M1)</f>
+        <v>Pin,Digital voltage card,Loopback PCB,LED,ADC card</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -718,8 +857,13 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>36</v>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G16" si="0">_xlfn.CONCAT(A2,",",B2,",",C2,",",D2,",",E2)</f>
+        <v>1,VIN,24V,24V,</v>
       </c>
       <c r="I2" s="1">
         <v>1</v>
@@ -730,37 +874,56 @@
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="5"/>
+      <c r="P2" s="8" t="str">
+        <f t="shared" ref="P2:P21" si="1">_xlfn.CONCAT(I2,",",J2,",",K2,",",L2,",",M2)</f>
+        <v>1,VIN,24V,24V,</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="0"/>
+        <v>2,DIG_IO_P1,PWM_G1,LED_G1_D6,AIN_A_P4</v>
       </c>
       <c r="I3" s="2">
         <v>2</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" t="s">
+        <v>91</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P3" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>2,DIG_IO_P14,PWM_G4,LED_G4_D6,AIN_A_P1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -770,23 +933,37 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="0"/>
+        <v>3,DIG_IO_P2,PWM_G7,LED_G7_D6,AIN_B_P2</v>
       </c>
       <c r="I4" s="1">
         <v>3</v>
       </c>
       <c r="J4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" t="s">
+        <v>92</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P4" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>3,DIG_IO_P15,PWM_G8,LED_G8_D6,AIN_B_P1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -796,23 +973,37 @@
       <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>4,DIG_IO_P3,PWM_G2,LED_G2_D6,AIN_A_P3</v>
       </c>
       <c r="I5" s="2">
         <v>4</v>
       </c>
       <c r="J5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" t="s">
+        <v>93</v>
+      </c>
+      <c r="M5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P5" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>4,DIG_IO_P16,PWM_G5,LED_G5_D6,AIN_B_P4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -822,23 +1013,33 @@
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>36</v>
+      <c r="D6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>5,DIG_IO_P4,PWM_G9,LED_G9_D6,</v>
       </c>
       <c r="I6" s="1">
         <v>5</v>
       </c>
       <c r="J6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="K6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L6" t="s">
+        <v>94</v>
+      </c>
+      <c r="M6" s="5"/>
+      <c r="P6" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>5,DIG_IO_P17,PWM_G11,LED_G11_D6,</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -848,23 +1049,37 @@
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>18</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>6,DIG_IO_P5,PWM_G3,LED_G3_D6,AIN_A_P2</v>
       </c>
       <c r="I7" s="2">
         <v>6</v>
       </c>
       <c r="J7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="L7" t="s">
+        <v>95</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="P7" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>6,DIG_IO_P18,PWM_G6,LED_G6_D6,AIN_B_P3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -874,23 +1089,33 @@
       <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>36</v>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>7,DIG_IO_P6,PWM_G10,LED_G10_D6,</v>
       </c>
       <c r="I8" s="1">
         <v>7</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" t="s">
+        <v>96</v>
+      </c>
+      <c r="M8" s="5"/>
+      <c r="P8" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>7,DIG_IO_P19,PWM_G12,LED_G12_D6,</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -900,23 +1125,33 @@
       <c r="C9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>36</v>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>8,DIG_IO_P7,IO_P1,LED1_D5,</v>
       </c>
       <c r="I9" s="2">
         <v>8</v>
       </c>
       <c r="J9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K9" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L9" t="s">
+        <v>97</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="P9" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>8,DIG_IO_P20,IO_P8,LED8_D5,</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -926,23 +1161,33 @@
       <c r="C10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>36</v>
+      <c r="D10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>9,DIG_IO_P8,IO_P2,LED2_D5,</v>
       </c>
       <c r="I10" s="1">
         <v>9</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L10" t="s">
+        <v>98</v>
+      </c>
+      <c r="M10" s="5"/>
+      <c r="P10" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>9,DIG_IO_P21,IO_P9,LED9_D5,</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -952,23 +1197,33 @@
       <c r="C11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>36</v>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>10,15V,15V,15V,</v>
       </c>
       <c r="I11" s="2">
         <v>10</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="L11" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="6"/>
+      <c r="P11" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>10,3V3,3V3,3V3,</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -978,23 +1233,33 @@
       <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>36</v>
+      <c r="D12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="5"/>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>11,DIG_IO_P9,IO_P3,LED3_D5,</v>
       </c>
       <c r="I12" s="1">
         <v>11</v>
       </c>
       <c r="J12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L12" t="s">
+        <v>99</v>
+      </c>
+      <c r="M12" s="5"/>
+      <c r="P12" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>11,DIG_IO_P22,IO_P10,LED10_D5,</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1004,23 +1269,33 @@
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>36</v>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>12,DIG_IO_P10,IO_P4,LED4_D5,</v>
       </c>
       <c r="I13" s="2">
         <v>12</v>
       </c>
       <c r="J13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L13" t="s">
+        <v>100</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="P13" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>12,DIG_IO_P23,IO_P11,LED11_D5,</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1030,23 +1305,33 @@
       <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>36</v>
+      <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>13,DIG_IO_P11,IO_P5,LED5_D5,</v>
       </c>
       <c r="I14" s="1">
         <v>13</v>
       </c>
       <c r="J14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K14" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L14" t="s">
+        <v>101</v>
+      </c>
+      <c r="M14" s="5"/>
+      <c r="P14" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>13,DIG_IO_P24,IO_P12,LED12_D5,</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1056,23 +1341,33 @@
       <c r="C15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>36</v>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>14,DIG_IO_P12,IO_P6,LED6_D5,</v>
       </c>
       <c r="I15" s="2">
         <v>14</v>
       </c>
       <c r="J15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="K15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L15" t="s">
+        <v>102</v>
+      </c>
+      <c r="M15" s="6"/>
+      <c r="P15" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>14,DIG_IO_P25,IO_P13,LED13_D5,</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1082,93 +1377,129 @@
       <c r="C16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>36</v>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>15,DIG_IO_P13,IO_P7,LED7_D5,</v>
       </c>
       <c r="I16" s="1">
         <v>15</v>
       </c>
       <c r="J16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="K16" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="9:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L16" t="s">
+        <v>103</v>
+      </c>
+      <c r="M16" s="5"/>
+      <c r="P16" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>15,DIG_IO_P26,IO_P14,LED14_D5,</v>
+      </c>
+    </row>
+    <row r="17" spans="9:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I17" s="2">
         <v>16</v>
       </c>
       <c r="J17" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="K17" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="K17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="9:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L17" t="s">
+        <v>104</v>
+      </c>
+      <c r="M17" s="6"/>
+      <c r="P17" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>16,DIG_IO_P27,IO_P15,LED15_D5,</v>
+      </c>
+    </row>
+    <row r="18" spans="9:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I18" s="1">
         <v>17</v>
       </c>
       <c r="J18" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="K18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L18" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="9:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L18" t="s">
+        <v>105</v>
+      </c>
+      <c r="M18" s="5"/>
+      <c r="P18" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>17,DIG_IO_P28,IO_P16,LED16_D5,</v>
+      </c>
+    </row>
+    <row r="19" spans="9:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I19" s="2">
         <v>18</v>
       </c>
       <c r="J19" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="K19" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="9:12" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L19" t="s">
+        <v>106</v>
+      </c>
+      <c r="M19" s="6"/>
+      <c r="P19" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>18,DIG_IO_P29,IO_P17,LED17_D5,</v>
+      </c>
+    </row>
+    <row r="20" spans="9:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I20" s="1">
         <v>19</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="L20" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="9:12" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L20" t="s">
+        <v>107</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="P20" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>19,DIG_IO_P30,IO_P18,LED18_D5,</v>
+      </c>
+    </row>
+    <row r="21" spans="9:16" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I21" s="2">
         <v>20</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="L21" s="6" t="s">
-        <v>36</v>
+        <v>75</v>
+      </c>
+      <c r="L21" t="s">
+        <v>75</v>
+      </c>
+      <c r="M21" s="6"/>
+      <c r="P21" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>20,5V,5V,5V,</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>